<commit_message>
calc for ifr and infections
</commit_message>
<xml_diff>
--- a/ref/Altersverteilung2.xlsx
+++ b/ref/Altersverteilung2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="120">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -326,9 +326,6 @@
     <t>Gestorbene bis KW 13/2021</t>
   </si>
   <si>
-    <t>Fälle bis KW/13/2012</t>
-  </si>
-  <si>
     <t>Altergruppe</t>
   </si>
   <si>
@@ -339,15 +336,51 @@
   </si>
   <si>
     <t>CFR (%)</t>
+  </si>
+  <si>
+    <t>80+</t>
+  </si>
+  <si>
+    <t>IF (%)</t>
+  </si>
+  <si>
+    <t>Infektionen</t>
+  </si>
+  <si>
+    <t>A00-A09</t>
+  </si>
+  <si>
+    <t>A10-A19</t>
+  </si>
+  <si>
+    <t>A20-A29</t>
+  </si>
+  <si>
+    <t>A30-A39</t>
+  </si>
+  <si>
+    <t>A40-A49</t>
+  </si>
+  <si>
+    <t>A50-A59</t>
+  </si>
+  <si>
+    <t>A60-A69</t>
+  </si>
+  <si>
+    <t>A70-A79</t>
+  </si>
+  <si>
+    <t>A80+</t>
+  </si>
+  <si>
+    <t>Altersverteilung in Deutschland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -905,7 +938,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -924,7 +957,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1280,13 +1319,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL44"/>
+  <dimension ref="A1:BL47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5397,23 +5439,49 @@
         <v>102</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="H25" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
+      <c r="K25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>104</v>
+      </c>
       <c r="M25" s="16"/>
+      <c r="N25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="T25" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -5442,8 +5510,21 @@
         <f>SUM(B3:BF3)</f>
         <v>70889</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="18"/>
+      <c r="K26" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L26" s="20">
+        <f>SUM(I26:I28)</f>
+        <v>265508</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="9"/>
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -5472,8 +5553,41 @@
         <f>SUM(B4:BF4)</f>
         <v>84511</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="18"/>
+      <c r="K27" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" s="20">
+        <f>I29</f>
+        <v>84997</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="8">
+        <f>SUM(C26:C27)</f>
+        <v>53072</v>
+      </c>
+      <c r="Q27" s="7">
+        <f>SUM(D26:D27)</f>
+        <v>265508</v>
+      </c>
+      <c r="R27" s="7">
+        <f>P27/Q27</f>
+        <v>0.19988851560028323</v>
+      </c>
+      <c r="S27" s="7">
+        <f>R27*100</f>
+        <v>19.988851560028323</v>
+      </c>
+      <c r="T27" s="7">
+        <f>(P27/$P$36)*(0.65/V41)</f>
+        <v>6.2845159953626402</v>
+      </c>
+      <c r="U27" s="9">
+        <f>ROUND((100 * P36 *V41 / 0.65), 0)</f>
+        <v>844488</v>
+      </c>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -5502,8 +5616,41 @@
         <f>SUM(B5:BF5)</f>
         <v>110108</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="7"/>
+      <c r="K28" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" s="20">
+        <f t="shared" ref="L28:L42" si="2">I30</f>
+        <v>81669</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="8">
+        <f>C28</f>
+        <v>14997</v>
+      </c>
+      <c r="Q28" s="7">
+        <f>D28</f>
+        <v>166666</v>
+      </c>
+      <c r="R28" s="7">
+        <f t="shared" ref="R28:R36" si="3">P28/Q28</f>
+        <v>8.9982359929439718E-2</v>
+      </c>
+      <c r="S28" s="7">
+        <f t="shared" ref="S28:S36" si="4">R28*100</f>
+        <v>8.9982359929439717</v>
+      </c>
+      <c r="T28" s="7">
+        <f>(P28/$P$36)*(0.65/U41)</f>
+        <v>1.4177227625477473</v>
+      </c>
+      <c r="U28" s="9">
+        <f>ROUND((100 * P36 *U41 / 0.65), 0)</f>
+        <v>1057823</v>
+      </c>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -5529,11 +5676,44 @@
         <v>68</v>
       </c>
       <c r="I29" s="9">
-        <f t="shared" ref="I29:I44" si="2">SUM(B6:BF6)</f>
+        <f t="shared" ref="I29:I44" si="5">SUM(B6:BF6)</f>
         <v>84997</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="7"/>
+      <c r="K29" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L29" s="20">
+        <f t="shared" si="2"/>
+        <v>101550</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="O29" s="7"/>
+      <c r="P29" s="8">
+        <f t="shared" ref="P29:P35" si="6">C29</f>
+        <v>6075</v>
+      </c>
+      <c r="Q29" s="7">
+        <f t="shared" ref="Q29:Q35" si="7">D29</f>
+        <v>273264</v>
+      </c>
+      <c r="R29" s="7">
+        <f t="shared" si="3"/>
+        <v>2.223124890216055E-2</v>
+      </c>
+      <c r="S29" s="7">
+        <f t="shared" si="4"/>
+        <v>2.223124890216055</v>
+      </c>
+      <c r="T29" s="7">
+        <f>(P29/$P$36)*(0.65/T41)</f>
+        <v>0.39846970743936388</v>
+      </c>
+      <c r="U29" s="9">
+        <f>ROUND((100 * P36 *T41 / 0.65), 0)</f>
+        <v>1524583</v>
+      </c>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -5559,11 +5739,44 @@
         <v>69</v>
       </c>
       <c r="I30" s="9">
+        <f t="shared" si="5"/>
+        <v>81669</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="L30" s="20">
         <f t="shared" si="2"/>
-        <v>81669</v>
-      </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="7"/>
+        <v>171714</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="O30" s="7"/>
+      <c r="P30" s="8">
+        <f t="shared" si="6"/>
+        <v>2085</v>
+      </c>
+      <c r="Q30" s="7">
+        <f t="shared" si="7"/>
+        <v>486412</v>
+      </c>
+      <c r="R30" s="7">
+        <f t="shared" si="3"/>
+        <v>4.2864896425252666E-3</v>
+      </c>
+      <c r="S30" s="7">
+        <f t="shared" si="4"/>
+        <v>0.42864896425252663</v>
+      </c>
+      <c r="T30" s="7">
+        <f>(P30/$P$36)*(0.65/S41)</f>
+        <v>0.11016360922104824</v>
+      </c>
+      <c r="U30" s="9">
+        <f>ROUND((100 * P36 *S41 / 0.65), 0)</f>
+        <v>1892640</v>
+      </c>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -5589,11 +5802,44 @@
         <v>70</v>
       </c>
       <c r="I31" s="9">
+        <f t="shared" si="5"/>
+        <v>101550</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="20">
         <f t="shared" si="2"/>
-        <v>101550</v>
-      </c>
-      <c r="K31" s="17"/>
-      <c r="L31" s="7"/>
+        <v>239945</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="O31" s="7"/>
+      <c r="P31" s="8">
+        <f t="shared" si="6"/>
+        <v>441</v>
+      </c>
+      <c r="Q31" s="7">
+        <f t="shared" si="7"/>
+        <v>411075</v>
+      </c>
+      <c r="R31" s="7">
+        <f t="shared" si="3"/>
+        <v>1.0727969348659004E-3</v>
+      </c>
+      <c r="S31" s="7">
+        <f t="shared" si="4"/>
+        <v>0.10727969348659004</v>
+      </c>
+      <c r="T31" s="7">
+        <f>(P31/$P$36)*(0.65/S41)</f>
+        <v>2.3300792166178551E-2</v>
+      </c>
+      <c r="U31" s="9">
+        <f>ROUND((100 * P36 *R41 / 0.65), 0)</f>
+        <v>1432616</v>
+      </c>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -5619,13 +5865,46 @@
         <v>71</v>
       </c>
       <c r="I32" s="9">
+        <f t="shared" si="5"/>
+        <v>171714</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="20">
         <f t="shared" si="2"/>
-        <v>171714</v>
-      </c>
-      <c r="K32" s="17"/>
-      <c r="L32" s="7"/>
+        <v>246467</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O32" s="7"/>
+      <c r="P32" s="8">
+        <f t="shared" si="6"/>
+        <v>149</v>
+      </c>
+      <c r="Q32" s="7">
+        <f t="shared" si="7"/>
+        <v>439015</v>
+      </c>
+      <c r="R32" s="7">
+        <f t="shared" si="3"/>
+        <v>3.3939614819539194E-4</v>
+      </c>
+      <c r="S32" s="7">
+        <f t="shared" si="4"/>
+        <v>3.3939614819539193E-2</v>
+      </c>
+      <c r="T32" s="7">
+        <f>(P32/$P$36)*(0.65/Q41)</f>
+        <v>9.6340808867833739E-3</v>
+      </c>
+      <c r="U32" s="9">
+        <f>ROUND((100 * P36 *Q41 / 0.65), 0)</f>
+        <v>1546593</v>
+      </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>99</v>
       </c>
@@ -5649,13 +5928,46 @@
         <v>72</v>
       </c>
       <c r="I33" s="9">
+        <f t="shared" si="5"/>
+        <v>239945</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" s="20">
         <f t="shared" si="2"/>
-        <v>239945</v>
-      </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="7"/>
+        <v>208676</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O33" s="7"/>
+      <c r="P33" s="8">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+      <c r="Q33" s="7">
+        <f t="shared" si="7"/>
+        <v>450001</v>
+      </c>
+      <c r="R33" s="7">
+        <f t="shared" si="3"/>
+        <v>1.1777751604996434E-4</v>
+      </c>
+      <c r="S33" s="7">
+        <f t="shared" si="4"/>
+        <v>1.1777751604996434E-2</v>
+      </c>
+      <c r="T33" s="7">
+        <f>(P33/$P$36)*(0.65/P41)</f>
+        <v>3.9286419727716506E-3</v>
+      </c>
+      <c r="U33" s="9">
+        <f>ROUND((100 * P36 *P41 / 0.65), 0)</f>
+        <v>1349067</v>
+      </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>101</v>
       </c>
@@ -5679,13 +5991,46 @@
         <v>73</v>
       </c>
       <c r="I34" s="9">
+        <f t="shared" si="5"/>
+        <v>246467</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="20">
         <f t="shared" si="2"/>
-        <v>246467</v>
-      </c>
-      <c r="K34" s="17"/>
-      <c r="L34" s="7"/>
+        <v>202399</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="O34" s="7"/>
+      <c r="P34" s="8">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="Q34" s="7">
+        <f t="shared" si="7"/>
+        <v>255943</v>
+      </c>
+      <c r="R34" s="7">
+        <f t="shared" si="3"/>
+        <v>2.3442719668051091E-5</v>
+      </c>
+      <c r="S34" s="7">
+        <f t="shared" si="4"/>
+        <v>2.3442719668051093E-3</v>
+      </c>
+      <c r="T34" s="7">
+        <f>(P34/$P$36)*(0.65/O41)</f>
+        <v>5.5629743414118934E-4</v>
+      </c>
+      <c r="U34" s="9">
+        <f>ROUND((100 * P36 *O41 / 0.65), 0)</f>
+        <v>1078560</v>
+      </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>100</v>
       </c>
@@ -5709,99 +6054,378 @@
         <v>74</v>
       </c>
       <c r="I35" s="9">
+        <f t="shared" si="5"/>
+        <v>208676</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L35" s="20">
         <f t="shared" si="2"/>
-        <v>208676</v>
-      </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="7"/>
+        <v>208232</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O35" s="11"/>
+      <c r="P35" s="12">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="Q35" s="11">
+        <f t="shared" si="7"/>
+        <v>146219</v>
+      </c>
+      <c r="R35" s="11">
+        <f t="shared" si="3"/>
+        <v>8.206867780520999E-5</v>
+      </c>
+      <c r="S35" s="11">
+        <f t="shared" si="4"/>
+        <v>8.2068677805209982E-3</v>
+      </c>
+      <c r="T35" s="11">
+        <f>(P35/$P$36)*(0.65/N41)</f>
+        <v>1.0880778180927257E-3</v>
+      </c>
+      <c r="U35" s="13">
+        <f>ROUND((100 * P36 *N41 / 0.65), 0)</f>
+        <v>1102862</v>
+      </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H36" s="14" t="s">
         <v>75</v>
       </c>
       <c r="I36" s="9">
+        <f t="shared" si="5"/>
+        <v>202399</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="L36" s="20">
         <f t="shared" si="2"/>
-        <v>202399</v>
+        <v>230783</v>
+      </c>
+      <c r="P36" s="23">
+        <f>SUM(P27:P35)</f>
+        <v>76890</v>
+      </c>
+      <c r="Q36" s="18">
+        <f>SUM(Q27:Q35)</f>
+        <v>2894103</v>
+      </c>
+      <c r="R36" s="18">
+        <f t="shared" si="3"/>
+        <v>2.6567817385905062E-2</v>
+      </c>
+      <c r="S36" s="18">
+        <f t="shared" si="4"/>
+        <v>2.6567817385905061</v>
+      </c>
+      <c r="T36">
+        <f>P36/U36*100</f>
+        <v>0.64999993237092657</v>
+      </c>
+      <c r="U36">
+        <f>SUM(U27:U35)</f>
+        <v>11829232</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="14" t="s">
         <v>76</v>
       </c>
       <c r="I37" s="9">
+        <f t="shared" si="5"/>
+        <v>208232</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L37" s="20">
         <f t="shared" si="2"/>
-        <v>208232</v>
+        <v>224588</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="H38" s="14" t="s">
         <v>77</v>
       </c>
       <c r="I38" s="9">
+        <f t="shared" si="5"/>
+        <v>230783</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L38" s="20">
         <f t="shared" si="2"/>
-        <v>230783</v>
-      </c>
+        <v>225413</v>
+      </c>
+      <c r="N38" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
       <c r="H39" s="14" t="s">
         <v>78</v>
       </c>
       <c r="I39" s="9">
+        <f t="shared" si="5"/>
+        <v>224588</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" s="20">
         <f t="shared" si="2"/>
-        <v>224588</v>
-      </c>
+        <v>158272</v>
+      </c>
+      <c r="N39" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="P39" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="T39" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
       <c r="H40" s="14" t="s">
         <v>79</v>
       </c>
       <c r="I40" s="9">
+        <f t="shared" si="5"/>
+        <v>225413</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L40" s="20">
         <f t="shared" si="2"/>
-        <v>225413</v>
+        <v>97671</v>
+      </c>
+      <c r="N40" s="14">
+        <v>7752706</v>
+      </c>
+      <c r="O40" s="7">
+        <v>7581868</v>
+      </c>
+      <c r="P40" s="7">
+        <v>9483430</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>10871964</v>
+      </c>
+      <c r="R40" s="7">
+        <v>10070748</v>
+      </c>
+      <c r="S40" s="7">
+        <v>13304542</v>
+      </c>
+      <c r="T40" s="7">
+        <v>10717241</v>
+      </c>
+      <c r="U40" s="7">
+        <v>7436098</v>
+      </c>
+      <c r="V40" s="7">
+        <v>5936434</v>
+      </c>
+      <c r="W40" s="9">
+        <v>83155031</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
       <c r="H41" s="14" t="s">
         <v>80</v>
       </c>
       <c r="I41" s="9">
+        <f t="shared" si="5"/>
+        <v>158272</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L41" s="20">
         <f t="shared" si="2"/>
-        <v>158272</v>
+        <v>82310</v>
+      </c>
+      <c r="N41" s="15">
+        <v>9.3231953698628287E-2</v>
+      </c>
+      <c r="O41" s="11">
+        <v>9.1177501936112557E-2</v>
+      </c>
+      <c r="P41" s="11">
+        <v>0.11404517424808608</v>
+      </c>
+      <c r="Q41" s="11">
+        <v>0.13074331004698922</v>
+      </c>
+      <c r="R41" s="11">
+        <v>0.12110810228667944</v>
+      </c>
+      <c r="S41" s="11">
+        <v>0.15999683771388409</v>
+      </c>
+      <c r="T41" s="11">
+        <v>0.12888265293292958</v>
+      </c>
+      <c r="U41" s="11">
+        <v>8.9424511188024206E-2</v>
+      </c>
+      <c r="V41" s="11">
+        <v>7.1389955948666539E-2</v>
+      </c>
+      <c r="W41" s="13">
+        <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
       <c r="H42" s="6" t="s">
         <v>82</v>
       </c>
       <c r="I42" s="9">
+        <f t="shared" si="5"/>
+        <v>97671</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L42" s="21">
         <f t="shared" si="2"/>
-        <v>97671</v>
+        <v>63909</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
       <c r="H43" s="6" t="s">
         <v>83</v>
       </c>
       <c r="I43" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>82310</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
       <c r="H44" s="15" t="s">
         <v>81</v>
       </c>
       <c r="I44" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>63909</v>
       </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A34 A19" twoDigitTextYear="1"/>
-    <ignoredError sqref="I27:I44" formulaRange="1"/>
+    <ignoredError sqref="A34 A19 K40 H42" twoDigitTextYear="1"/>
+    <ignoredError sqref="I26:I44" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>